<commit_message>
returning data from datastore as json
</commit_message>
<xml_diff>
--- a/bnsworkplan.xlsx
+++ b/bnsworkplan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="132">
   <si>
     <t>מצוינות בשרות לתושב</t>
   </si>
@@ -65,9 +65,6 @@
     <t>מנהלת לשכה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2018</t>
-  </si>
-  <si>
     <t>הבטחת רמת השירות לתושב עקב שינויים צפויים בגבולות המועצה</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>השתתפות בכל ישיבות הוועדה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2019</t>
-  </si>
-  <si>
     <t>היערכות לקליטת כרמית, על פי החלטת הועדה</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>פרויקטורית, מנהלי אגפים</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2020</t>
-  </si>
-  <si>
     <t>פיתוח כלכלי של המועצה</t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t>מנכ"ל דודאים, חברה כלכלית, גזברית</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2021</t>
-  </si>
-  <si>
     <t>הגעה להסדר עם רשות המיסים על שומת דודאים</t>
   </si>
   <si>
@@ -125,9 +113,6 @@
     <t>גזברית, מנכ"לית</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2022</t>
-  </si>
-  <si>
     <t>מעורבות והשפעה בחברה והסביבה</t>
   </si>
   <si>
@@ -146,18 +131,12 @@
     <t>ע. ראש המועצה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2023</t>
-  </si>
-  <si>
     <t>אירוח שרים, חכ"ים, מועצות אחרות בבני שמעון</t>
   </si>
   <si>
     <t>לפחות 6 ביקורים בשנה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2024</t>
-  </si>
-  <si>
     <t>תקשורת ומידע</t>
   </si>
   <si>
@@ -170,9 +149,6 @@
     <t>הוצאת הודעה לתקשורת/כתבה/ נאום/מכתב לפחות  30 במהלך השנה.</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2025</t>
-  </si>
-  <si>
     <t>הגדרת תכנית יח"צ למיתוג דודאים לשינוי התודעה הציבורית לגבי האתר</t>
   </si>
   <si>
@@ -182,9 +158,6 @@
     <t>צוות דודאים, צוות תקשורת, ע.ראש המועצה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2026</t>
-  </si>
-  <si>
     <t>קידום נושאים אזוריים ולאומיים</t>
   </si>
   <si>
@@ -200,9 +173,6 @@
     <t>מנכ"ל עידן הנגב</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2027</t>
-  </si>
-  <si>
     <t>מתחם תעסוקה שוקת</t>
   </si>
   <si>
@@ -212,21 +182,12 @@
     <t>חכ"ל</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2028</t>
-  </si>
-  <si>
     <t>מתחם לוגיסטי נבטים</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2029</t>
-  </si>
-  <si>
     <t>נגב פארק</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2030</t>
-  </si>
-  <si>
     <t>קידום האינטרסים המקומיים במרכז המועצות האזוריות</t>
   </si>
   <si>
@@ -236,9 +197,6 @@
     <t>השתתפות ב80% ישיבות הוועדה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2031</t>
-  </si>
-  <si>
     <t>פיתוח ווחיזוק הקהילה האיזורית</t>
   </si>
   <si>
@@ -257,18 +215,12 @@
     <t>צוות מטה</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2032</t>
-  </si>
-  <si>
     <t>מפגש הכנה בכל יישוב עד הבחירות</t>
   </si>
   <si>
     <t>1,2,3</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2033</t>
-  </si>
-  <si>
     <t>שיתוף פעולה עם הנהגות היישובים והתושבים</t>
   </si>
   <si>
@@ -281,9 +233,6 @@
     <t>2,3</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2034</t>
-  </si>
-  <si>
     <t>סדנת וועדים לשיתוף ציבור וקביעת סדר יומה של המועצה</t>
   </si>
   <si>
@@ -293,9 +242,6 @@
     <t>ראש מועצה חדש?</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2035</t>
-  </si>
-  <si>
     <t>המשך ביסוס אשכול נגב מערבי</t>
   </si>
   <si>
@@ -311,21 +257,12 @@
     <t>אשכול נגב ערבי</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2036</t>
-  </si>
-  <si>
     <t>הפעלת שירותי פינוי פסולת אזוריים</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2037</t>
-  </si>
-  <si>
     <t>הפעלת מיזמים חברתיים אזוריים</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2038</t>
-  </si>
-  <si>
     <t>המשך ביסוס פעילות כוכבי המדבר במועצה</t>
   </si>
   <si>
@@ -341,9 +278,6 @@
     <t>עמותת כוכבי המדבר</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2039</t>
-  </si>
-  <si>
     <t>ערי חינוך מחינוך איכותי למצוין</t>
   </si>
   <si>
@@ -362,9 +296,6 @@
     <t>הנדסה, חינוך, מנכלית, גזברית, מנהל בית הספר, מבקרת</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2040</t>
-  </si>
-  <si>
     <t>התחלת הקמת בית ספר עדנים</t>
   </si>
   <si>
@@ -374,9 +305,6 @@
     <t>צוות עדנים</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2041</t>
-  </si>
-  <si>
     <t>הגברת תחושת הביטחון של תושבי המועצה</t>
   </si>
   <si>
@@ -392,21 +320,12 @@
     <t xml:space="preserve">הנדסה, </t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2042</t>
-  </si>
-  <si>
     <t>צומת להבים</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2043</t>
-  </si>
-  <si>
     <t>הרחבת כביש 264</t>
   </si>
   <si>
-    <t>יעדים שוטפים / עדכון תכנית 2044</t>
-  </si>
-  <si>
     <t>שדרוג תחנות ההסעה ביישובים</t>
   </si>
   <si>
@@ -414,9 +333,6 @@
   </si>
   <si>
     <t>הנדסה, מנהל בטיחות</t>
-  </si>
-  <si>
-    <t>יעדים שוטפים / עדכון תכנית 2045</t>
   </si>
   <si>
     <t>שימור, יעול והגדלת הכנסות</t>
@@ -857,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE738190-3366-4865-AB17-7F0D64BE1094}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +858,7 @@
         <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -950,17 +866,17 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" t="s">
         <v>5</v>
       </c>
@@ -980,7 +896,7 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -988,57 +904,57 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
       <c r="N4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1059,30 +975,30 @@
         <v>6</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1100,150 +1016,150 @@
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" t="s">
-        <v>39</v>
-      </c>
       <c r="N7" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
       <c r="N8" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
       <c r="N9" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>5</v>
@@ -1264,27 +1180,27 @@
         <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="N10" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
         <v>5</v>
@@ -1305,27 +1221,27 @@
         <v>6</v>
       </c>
       <c r="L11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
@@ -1346,27 +1262,27 @@
         <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -1387,27 +1303,27 @@
         <v>6</v>
       </c>
       <c r="L13" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="N13" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -1428,27 +1344,27 @@
         <v>6</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="N14" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -1469,24 +1385,24 @@
         <v>6</v>
       </c>
       <c r="N15" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1507,30 +1423,30 @@
         <v>6</v>
       </c>
       <c r="L16" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="N16" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1548,30 +1464,30 @@
         <v>6</v>
       </c>
       <c r="L17" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1589,24 +1505,24 @@
         <v>6</v>
       </c>
       <c r="L18" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="N18" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F19">
         <v>4</v>
@@ -1621,30 +1537,30 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K19" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="N19" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
@@ -1665,27 +1581,27 @@
         <v>6</v>
       </c>
       <c r="L20" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="N20" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -1706,27 +1622,27 @@
         <v>6</v>
       </c>
       <c r="L21" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="N21" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
         <v>5</v>
@@ -1747,27 +1663,27 @@
         <v>6</v>
       </c>
       <c r="L22" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="N22" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
         <v>5</v>
@@ -1788,27 +1704,27 @@
         <v>6</v>
       </c>
       <c r="L23" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="N23" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
         <v>5</v>
@@ -1829,27 +1745,27 @@
         <v>6</v>
       </c>
       <c r="L24" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="N24" t="s">
-        <v>112</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="F25" t="s">
         <v>5</v>
@@ -1870,24 +1786,24 @@
         <v>6</v>
       </c>
       <c r="L25" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="N25" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="F26" t="s">
         <v>5</v>
@@ -1908,24 +1824,24 @@
         <v>6</v>
       </c>
       <c r="L26" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="N26" t="s">
-        <v>122</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
         <v>5</v>
@@ -1946,21 +1862,21 @@
         <v>6</v>
       </c>
       <c r="N27" t="s">
-        <v>124</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
         <v>5</v>
@@ -1981,21 +1897,21 @@
         <v>6</v>
       </c>
       <c r="N28" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="F29" t="s">
         <v>5</v>
@@ -2016,27 +1932,27 @@
         <v>6</v>
       </c>
       <c r="L29" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="N29" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="E30" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2057,27 +1973,27 @@
         <v>6</v>
       </c>
       <c r="L30" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="N30" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="E31" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2098,27 +2014,27 @@
         <v>6</v>
       </c>
       <c r="L31" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="N31" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2139,10 +2055,10 @@
         <v>6</v>
       </c>
       <c r="L32" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="N32" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2150,16 +2066,16 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C33" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="E33" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -2180,10 +2096,10 @@
         <v>6</v>
       </c>
       <c r="L33" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N33" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -2191,16 +2107,16 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C34" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="E34" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="F34">
         <v>3</v>
@@ -2221,10 +2137,10 @@
         <v>6</v>
       </c>
       <c r="L34" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="N34" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -2232,16 +2148,16 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E35" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="F35">
         <v>2</v>
@@ -2262,27 +2178,27 @@
         <v>6</v>
       </c>
       <c r="L35" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="N35" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="F36" t="s">
         <v>5</v>
@@ -2303,27 +2219,27 @@
         <v>6</v>
       </c>
       <c r="L36" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="N36" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="D37" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="F37" t="s">
         <v>5</v>
@@ -2344,10 +2260,10 @@
         <v>6</v>
       </c>
       <c r="L37" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="N37" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>